<commit_message>
cambios antes de hacer fetch
</commit_message>
<xml_diff>
--- a/public/ReportOut.xlsx
+++ b/public/ReportOut.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>Logo Arauco</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Sistema bloqueado:</t>
   </si>
   <si>
-    <t>vapor2</t>
+    <t>Agua Vapor</t>
   </si>
   <si>
     <t>Ito Planta Turno día:</t>
@@ -68,19 +68,19 @@
     <t>Inicio:</t>
   </si>
   <si>
-    <t>23/02/2017</t>
+    <t>24/02/2018</t>
   </si>
   <si>
     <t>Hora Inicio:</t>
   </si>
   <si>
-    <t>2017-03-23T15:50:57Z</t>
+    <t>2017-04-15T18:16:47Z</t>
   </si>
   <si>
     <t>Término:</t>
   </si>
   <si>
-    <t>24/02/2017</t>
+    <t>25/02/2018</t>
   </si>
   <si>
     <t>Hora Termino:</t>
@@ -110,15 +110,18 @@
     <t>Avance</t>
   </si>
   <si>
-    <t xml:space="preserve">Cambio de Caps (60cu) </t>
-  </si>
-  <si>
-    <t>Marcado de Caps</t>
+    <t>Reparacion estructural</t>
+  </si>
+  <si>
+    <t>trabajo 1</t>
   </si>
   <si>
     <t>100%</t>
   </si>
   <si>
+    <t>trabajo 2</t>
+  </si>
+  <si>
     <t>Observaciones</t>
   </si>
   <si>
@@ -128,7 +131,7 @@
     <t>1.-</t>
   </si>
   <si>
-    <t>nada que agregar</t>
+    <t>Ggggggg</t>
   </si>
   <si>
     <t>2.-</t>
@@ -654,7 +657,7 @@
   <dimension ref="A1:AMK45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1847,6 +1850,9 @@
     </row>
     <row r="21" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B21" s="7"/>
+      <c r="C21" s="21" t="s">
+        <v>34</v>
+      </c>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:1025" customHeight="1" ht="12.8">
@@ -1900,39 +1906,39 @@
     <row r="34" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B34" s="11"/>
       <c r="C34" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B35" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B36" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B37" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B38" s="13"/>
       <c r="C38" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -1940,13 +1946,13 @@
     </row>
     <row r="39" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B39" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F39" s="8"/>
     </row>
@@ -1958,13 +1964,13 @@
     </row>
     <row r="41" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B41" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F41" s="8"/>
     </row>

</xml_diff>